<commit_message>
Modifications sur la page d'accueil 	modified:   docs/Gestion du Projet.xlsx 	modified:   src/Easy/ArticleBundle/Controller/ArticleController.php 	modified:   src/Easy/ArticleBundle/Resources/config/routing.yml 	deleted:    src/Easy/ArticleBundle/Resources/views/Article/index.html.twig 	new file:   src/Easy/ArticleBundle/Resources/views/Article/listAdmin.html.twig 	modified:   src/Easy/EspaceMembreBundle/Resources/views/layout.html.twig 	modified:   src/Easy/SiteBundle/Resources/views/layout.html.twig
</commit_message>
<xml_diff>
--- a/docs/Gestion du Projet.xlsx
+++ b/docs/Gestion du Projet.xlsx
@@ -206,10 +206,10 @@
     <xf numFmtId="9" fontId="3" fillId="2" borderId="0" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="4" fillId="3" borderId="0" xfId="3" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="7" fillId="5" borderId="0" xfId="5" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="7" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="7" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Accent1" xfId="4" builtinId="29"/>
@@ -526,7 +526,7 @@
   <dimension ref="B1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -538,16 +538,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:4">
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
     </row>
     <row r="2" spans="2:4">
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
     </row>
     <row r="4" spans="2:4">
       <c r="B4" s="4" t="s">
@@ -639,8 +639,8 @@
       <c r="C13" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="8">
-        <v>0</v>
+      <c r="D13" s="7">
+        <v>0.6</v>
       </c>
     </row>
     <row r="14" spans="2:4">
@@ -650,8 +650,8 @@
       <c r="C14" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="8">
-        <v>0</v>
+      <c r="D14" s="7">
+        <v>0.2</v>
       </c>
     </row>
     <row r="15" spans="2:4">
@@ -716,7 +716,7 @@
       <c r="C20" t="s">
         <v>11</v>
       </c>
-      <c r="D20" s="10">
+      <c r="D20" s="9">
         <v>0</v>
       </c>
     </row>
@@ -732,7 +732,9 @@
       <c r="C22" t="s">
         <v>16</v>
       </c>
-      <c r="D22" s="1"/>
+      <c r="D22" s="7">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="23" spans="2:4">
       <c r="D23" s="1"/>

</xml_diff>